<commit_message>
Dodato ciscenje starih logova
</commit_message>
<xml_diff>
--- a/Power Distribution System/Power Distribution System/bin/Debug/hidro.xlsx
+++ b/Power Distribution System/Power Distribution System/bin/Debug/hidro.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>No.</t>
   </si>
@@ -26,21 +26,24 @@
     <t>1</t>
   </si>
   <si>
-    <t>08/01/2023 9:38:35 pm</t>
+    <t>08/01/2023 9:52:55 pm</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
+    <t>08/01/2023 9:52:56 pm</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
-    <t>08/01/2023 9:38:36 pm</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
+    <t>08/01/2023 9:52:57 pm</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
@@ -53,9 +56,6 @@
     <t>8</t>
   </si>
   <si>
-    <t>08/01/2023 9:38:37 pm</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
@@ -65,7 +65,7 @@
     <t>11</t>
   </si>
   <si>
-    <t>08/01/2023 9:38:38 pm</t>
+    <t>08/01/2023 9:52:58 pm</t>
   </si>
   <si>
     <t>12</t>
@@ -74,58 +74,40 @@
     <t>13</t>
   </si>
   <si>
-    <t>08/01/2023 9:38:39 pm</t>
-  </si>
-  <si>
     <t>14</t>
   </si>
   <si>
     <t>15</t>
   </si>
   <si>
-    <t>08/01/2023 9:38:40 pm</t>
-  </si>
-  <si>
     <t>16</t>
   </si>
   <si>
+    <t>08/01/2023 9:52:59 pm</t>
+  </si>
+  <si>
     <t>17</t>
   </si>
   <si>
     <t>18</t>
   </si>
   <si>
-    <t>08/01/2023 9:38:41 pm</t>
-  </si>
-  <si>
     <t>19</t>
   </si>
   <si>
+    <t>08/01/2023 9:53:01 pm</t>
+  </si>
+  <si>
     <t>20</t>
   </si>
   <si>
-    <t>08/01/2023 9:38:42 pm</t>
-  </si>
-  <si>
     <t>21</t>
   </si>
   <si>
+    <t>08/01/2023 9:53:02 pm</t>
+  </si>
+  <si>
     <t>22</t>
-  </si>
-  <si>
-    <t>08/01/2023 9:38:43 pm</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>08/01/2023 9:38:44 pm</t>
   </si>
 </sst>
 </file>
@@ -179,7 +161,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -217,7 +199,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" s="0">
         <v>6</v>
@@ -225,10 +207,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C4" s="0">
         <v>9</v>
@@ -239,7 +221,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" s="0">
         <v>12</v>
@@ -247,10 +229,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" s="0">
         <v>15</v>
@@ -258,10 +240,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7" s="0">
         <v>18</v>
@@ -269,10 +251,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C8" s="0">
         <v>21</v>
@@ -280,10 +262,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C9" s="0">
         <v>24</v>
@@ -294,7 +276,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C10" s="0">
         <v>27</v>
@@ -305,7 +287,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C11" s="0">
         <v>30</v>
@@ -338,7 +320,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C14" s="0">
         <v>39</v>
@@ -346,10 +328,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C15" s="0">
         <v>42</v>
@@ -357,10 +339,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C16" s="0">
         <v>45</v>
@@ -368,7 +350,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>23</v>
@@ -379,7 +361,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>23</v>
@@ -390,10 +372,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C19" s="0">
         <v>54</v>
@@ -401,7 +383,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>27</v>
@@ -412,10 +394,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C21" s="0">
         <v>60</v>
@@ -423,7 +405,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>30</v>
@@ -434,46 +416,13 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C23" s="0">
         <v>66</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="0">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="0">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="0">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dodato cuvanje u excel za solar i wind
</commit_message>
<xml_diff>
--- a/Power Distribution System/Power Distribution System/bin/Debug/hidro.xlsx
+++ b/Power Distribution System/Power Distribution System/bin/Debug/hidro.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>No.</t>
   </si>
@@ -26,61 +26,124 @@
     <t>1</t>
   </si>
   <si>
-    <t>9.1.2023. 15:03:49</t>
+    <t>09/01/2023 9:11:11 pm</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>9.1.2023. 15:03:52</t>
+    <t>09/01/2023 9:11:12 pm</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>9.1.2023. 15:03:53</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
-    <t>9.1.2023. 15:03:54</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
-    <t>9.1.2023. 15:03:55</t>
+    <t>09/01/2023 9:11:13 pm</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
-    <t>9.1.2023. 15:03:56</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
+    <t>09/01/2023 9:11:14 pm</t>
+  </si>
+  <si>
     <t>8</t>
   </si>
   <si>
-    <t>9.1.2023. 15:03:57</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>9.1.2023. 15:03:58</t>
+    <t>09/01/2023 9:11:15 pm</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
-    <t>9.1.2023. 15:03:59</t>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>09/01/2023 9:11:16 pm</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>09/01/2023 9:11:17 pm</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>09/01/2023 9:11:18 pm</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>09/01/2023 9:11:19 pm</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>09/01/2023 9:11:20 pm</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>09/01/2023 9:11:25 pm</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>09/01/2023 9:11:29 pm</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>09/01/2023 9:11:31 pm</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>09/01/2023 9:11:32 pm</t>
   </si>
 </sst>
 </file>
@@ -134,14 +197,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.1001957484654" customWidth="1"/>
+    <col min="2" max="2" width="21.5709904261998" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -183,7 +246,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="0">
         <v>0</v>
@@ -191,10 +254,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="0">
         <v>0</v>
@@ -202,10 +265,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="0">
         <v>0</v>
@@ -213,10 +276,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C7" s="0">
         <v>0</v>
@@ -224,57 +287,233 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C9" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C10" s="0">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C11" s="0">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="C14" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="0">
-        <v>0</v>
+      <c r="B15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="0">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="0">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dodata zastita u slucaju da hidroelektrana predje 100%
</commit_message>
<xml_diff>
--- a/Power Distribution System/Power Distribution System/bin/Debug/hidro.xlsx
+++ b/Power Distribution System/Power Distribution System/bin/Debug/hidro.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>No.</t>
   </si>
@@ -26,13 +26,13 @@
     <t>1</t>
   </si>
   <si>
-    <t>09/01/2023 9:11:11 pm</t>
+    <t>09/01/2023 11:16:03 pm</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>09/01/2023 9:11:12 pm</t>
+    <t>09/01/2023 11:16:04 pm</t>
   </si>
   <si>
     <t>3</t>
@@ -44,16 +44,13 @@
     <t>5</t>
   </si>
   <si>
-    <t>09/01/2023 9:11:13 pm</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>09/01/2023 9:11:14 pm</t>
+    <t>09/01/2023 11:16:05 pm</t>
   </si>
   <si>
     <t>8</t>
@@ -62,55 +59,61 @@
     <t>9</t>
   </si>
   <si>
+    <t>09/01/2023 11:16:06 pm</t>
+  </si>
+  <si>
     <t>10</t>
   </si>
   <si>
-    <t>09/01/2023 9:11:15 pm</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
+    <t>09/01/2023 11:16:07 pm</t>
+  </si>
+  <si>
     <t>13</t>
   </si>
   <si>
-    <t>09/01/2023 9:11:16 pm</t>
-  </si>
-  <si>
     <t>14</t>
   </si>
   <si>
+    <t>09/01/2023 11:16:08 pm</t>
+  </si>
+  <si>
     <t>15</t>
   </si>
   <si>
     <t>16</t>
   </si>
   <si>
-    <t>09/01/2023 9:11:17 pm</t>
+    <t>09/01/2023 11:16:09 pm</t>
   </si>
   <si>
     <t>17</t>
   </si>
   <si>
+    <t>09/01/2023 11:16:10 pm</t>
+  </si>
+  <si>
     <t>18</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>09/01/2023 9:11:18 pm</t>
-  </si>
-  <si>
     <t>20</t>
   </si>
   <si>
+    <t>09/01/2023 11:16:11 pm</t>
+  </si>
+  <si>
     <t>21</t>
   </si>
   <si>
-    <t>09/01/2023 9:11:19 pm</t>
+    <t>09/01/2023 11:16:12 pm</t>
   </si>
   <si>
     <t>22</t>
@@ -119,31 +122,43 @@
     <t>23</t>
   </si>
   <si>
-    <t>09/01/2023 9:11:20 pm</t>
+    <t>09/01/2023 11:16:13 pm</t>
   </si>
   <si>
     <t>24</t>
   </si>
   <si>
-    <t>09/01/2023 9:11:25 pm</t>
-  </si>
-  <si>
     <t>25</t>
   </si>
   <si>
-    <t>09/01/2023 9:11:29 pm</t>
+    <t>09/01/2023 11:16:14 pm</t>
   </si>
   <si>
     <t>26</t>
   </si>
   <si>
-    <t>09/01/2023 9:11:31 pm</t>
-  </si>
-  <si>
     <t>27</t>
   </si>
   <si>
-    <t>09/01/2023 9:11:32 pm</t>
+    <t>09/01/2023 11:16:15 pm</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>09/01/2023 11:16:16 pm</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>09/01/2023 11:16:17 pm</t>
   </si>
 </sst>
 </file>
@@ -197,14 +212,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.5709904261998" customWidth="1"/>
+    <col min="2" max="2" width="22.6646466936384" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -268,7 +283,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C6" s="0">
         <v>0</v>
@@ -276,10 +291,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" s="0">
         <v>0</v>
@@ -287,10 +302,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>13</v>
       </c>
       <c r="C8" s="0">
         <v>1</v>
@@ -298,10 +313,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="0">
         <v>4</v>
@@ -309,10 +324,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>13</v>
       </c>
       <c r="C10" s="0">
         <v>7</v>
@@ -323,7 +338,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="0">
         <v>10</v>
@@ -331,10 +346,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" s="0">
         <v>13</v>
@@ -342,10 +357,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="C13" s="0">
         <v>16</v>
@@ -356,7 +371,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="0">
         <v>19</v>
@@ -364,10 +379,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>21</v>
       </c>
       <c r="C15" s="0">
         <v>22</v>
@@ -378,7 +393,7 @@
         <v>23</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="0">
         <v>25</v>
@@ -400,7 +415,7 @@
         <v>26</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C18" s="0">
         <v>31</v>
@@ -408,10 +423,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>25</v>
       </c>
       <c r="C19" s="0">
         <v>34</v>
@@ -419,10 +434,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="0">
         <v>37</v>
@@ -433,7 +448,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C21" s="0">
         <v>40</v>
@@ -441,10 +456,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C22" s="0">
         <v>43</v>
@@ -452,10 +467,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>32</v>
       </c>
       <c r="C23" s="0">
         <v>46</v>
@@ -463,10 +478,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C24" s="0">
         <v>49</v>
@@ -474,10 +489,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>37</v>
       </c>
       <c r="C25" s="0">
         <v>52</v>
@@ -499,7 +514,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C27" s="0">
         <v>58</v>
@@ -507,13 +522,57 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="C28" s="0">
         <v>61</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="0">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="0">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="0">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>